<commit_message>
Daily status - 2/21 - Yash
</commit_message>
<xml_diff>
--- a/Daily_Status_Update.xlsx
+++ b/Daily_Status_Update.xlsx
@@ -107,8 +107,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,7 +389,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -413,24 +413,24 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -459,7 +459,7 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.1</v>
       </c>
     </row>
@@ -467,8 +467,8 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="C8" s="3">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>